<commit_message>
Updated data (Strava) and all figures.
</commit_message>
<xml_diff>
--- a/data/raw/strava_year.xlsx
+++ b/data/raw/strava_year.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="60">
   <si>
     <t>timeframe</t>
   </si>
@@ -123,6 +123,72 @@
     <t>S Fork Flathead Creek</t>
   </si>
   <si>
+    <t>subsectionname</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Steep Way</t>
+  </si>
+  <si>
+    <t>College M to Sypes</t>
+  </si>
+  <si>
+    <t>M to Baldy</t>
+  </si>
+  <si>
+    <t>Sypes to Middle Cottonwood</t>
+  </si>
+  <si>
+    <t>Middle Cottonwood to Bostwick</t>
+  </si>
+  <si>
+    <t>Baldy to Bridger</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Bridger</t>
+  </si>
+  <si>
+    <t>Bostwick to Truman</t>
+  </si>
+  <si>
+    <t>Truman to Jones</t>
+  </si>
+  <si>
+    <t>Ross Pass to Sacagawea Peak</t>
+  </si>
+  <si>
+    <t>Jones to Ross Pass</t>
+  </si>
+  <si>
+    <t>Bridger to Ross Pass</t>
+  </si>
+  <si>
+    <t>North Cottonwood to Ridge</t>
+  </si>
+  <si>
+    <t>North Cottonwood to Johnson Canyon</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Ross Pass to Sacagawea Pass</t>
+  </si>
+  <si>
+    <t>Sacagawea Peak to Sacagawea Pass</t>
+  </si>
+  <si>
+    <t>Upper Shafthouse</t>
+  </si>
+  <si>
+    <t>Lower Shafthouse</t>
+  </si>
+  <si>
     <t>totaltrips</t>
   </si>
   <si>
@@ -189,7 +255,10 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2">
@@ -205,10 +274,13 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="0">
         <v>330</v>
       </c>
-      <c r="F2" s="0">
+      <c r="G2" s="0">
         <v>305</v>
       </c>
     </row>
@@ -225,12 +297,15 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="0">
-        <v>20</v>
+      <c r="E3" t="s">
+        <v>37</v>
       </c>
       <c r="F3" s="0">
         <v>20</v>
       </c>
+      <c r="G3" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -245,12 +320,15 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="0">
-        <v>20</v>
+      <c r="E4" t="s">
+        <v>37</v>
       </c>
       <c r="F4" s="0">
         <v>20</v>
       </c>
+      <c r="G4" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -265,10 +343,13 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="0">
         <v>510</v>
       </c>
-      <c r="F5" s="0">
+      <c r="G5" s="0">
         <v>450</v>
       </c>
     </row>
@@ -285,10 +366,13 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="0">
         <v>575</v>
       </c>
-      <c r="F6" s="0">
+      <c r="G6" s="0">
         <v>505</v>
       </c>
     </row>
@@ -305,10 +389,13 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="0">
         <v>685</v>
       </c>
-      <c r="F7" s="0">
+      <c r="G7" s="0">
         <v>590</v>
       </c>
     </row>
@@ -325,10 +412,13 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="0">
         <v>14500</v>
       </c>
-      <c r="F8" s="0">
+      <c r="G8" s="0">
         <v>4430</v>
       </c>
     </row>
@@ -345,10 +435,13 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="0">
         <v>7675</v>
       </c>
-      <c r="F9" s="0">
+      <c r="G9" s="0">
         <v>2465</v>
       </c>
     </row>
@@ -365,10 +458,13 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="0">
         <v>14165</v>
       </c>
-      <c r="F10" s="0">
+      <c r="G10" s="0">
         <v>4325</v>
       </c>
     </row>
@@ -385,10 +481,13 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="0">
         <v>12190</v>
       </c>
-      <c r="F11" s="0">
+      <c r="G11" s="0">
         <v>3530</v>
       </c>
     </row>
@@ -405,10 +504,13 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="0">
         <v>1005</v>
       </c>
-      <c r="F12" s="0">
+      <c r="G12" s="0">
         <v>745</v>
       </c>
     </row>
@@ -425,10 +527,13 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="0">
         <v>2040</v>
       </c>
-      <c r="F13" s="0">
+      <c r="G13" s="0">
         <v>1245</v>
       </c>
     </row>
@@ -445,10 +550,13 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="0">
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="0">
         <v>6915</v>
       </c>
-      <c r="F14" s="0">
+      <c r="G14" s="0">
         <v>2225</v>
       </c>
     </row>
@@ -465,10 +573,13 @@
       <c r="D15" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="0">
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="0">
         <v>2655</v>
       </c>
-      <c r="F15" s="0">
+      <c r="G15" s="0">
         <v>1690</v>
       </c>
     </row>
@@ -485,10 +596,13 @@
       <c r="D16" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="0">
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="0">
         <v>10440</v>
       </c>
-      <c r="F16" s="0">
+      <c r="G16" s="0">
         <v>3590</v>
       </c>
     </row>
@@ -505,10 +619,13 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="0">
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="0">
         <v>6535</v>
       </c>
-      <c r="F17" s="0">
+      <c r="G17" s="0">
         <v>2260</v>
       </c>
     </row>
@@ -525,10 +642,13 @@
       <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="0">
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="0">
         <v>1370</v>
       </c>
-      <c r="F18" s="0">
+      <c r="G18" s="0">
         <v>975</v>
       </c>
     </row>
@@ -545,10 +665,13 @@
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="0">
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="0">
         <v>8695</v>
       </c>
-      <c r="F19" s="0">
+      <c r="G19" s="0">
         <v>2810</v>
       </c>
     </row>
@@ -565,10 +688,13 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="0">
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="0">
         <v>4400</v>
       </c>
-      <c r="F20" s="0">
+      <c r="G20" s="0">
         <v>1495</v>
       </c>
     </row>
@@ -585,10 +711,13 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="0">
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="0">
         <v>1265</v>
       </c>
-      <c r="F21" s="0">
+      <c r="G21" s="0">
         <v>520</v>
       </c>
     </row>
@@ -605,10 +734,13 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="0">
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="0">
         <v>4840</v>
       </c>
-      <c r="F22" s="0">
+      <c r="G22" s="0">
         <v>2210</v>
       </c>
     </row>
@@ -625,10 +757,13 @@
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="0">
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="0">
         <v>4755</v>
       </c>
-      <c r="F23" s="0">
+      <c r="G23" s="0">
         <v>2095</v>
       </c>
     </row>
@@ -645,10 +780,13 @@
       <c r="D24" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="0">
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="0">
         <v>4460</v>
       </c>
-      <c r="F24" s="0">
+      <c r="G24" s="0">
         <v>2410</v>
       </c>
     </row>
@@ -665,10 +803,13 @@
       <c r="D25" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="0">
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="0">
         <v>2925</v>
       </c>
-      <c r="F25" s="0">
+      <c r="G25" s="0">
         <v>1695</v>
       </c>
     </row>
@@ -685,10 +826,13 @@
       <c r="D26" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="0">
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="0">
         <v>4005</v>
       </c>
-      <c r="F26" s="0">
+      <c r="G26" s="0">
         <v>2225</v>
       </c>
     </row>
@@ -705,10 +849,13 @@
       <c r="D27" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="0">
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="0">
         <v>4405</v>
       </c>
-      <c r="F27" s="0">
+      <c r="G27" s="0">
         <v>2415</v>
       </c>
     </row>
@@ -725,10 +872,13 @@
       <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="0">
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="0">
         <v>4425</v>
       </c>
-      <c r="F28" s="0">
+      <c r="G28" s="0">
         <v>2420</v>
       </c>
     </row>
@@ -745,10 +895,13 @@
       <c r="D29" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="0">
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="0">
         <v>3865</v>
       </c>
-      <c r="F29" s="0">
+      <c r="G29" s="0">
         <v>1340</v>
       </c>
     </row>
@@ -765,10 +918,13 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="0">
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="0">
         <v>2075</v>
       </c>
-      <c r="F30" s="0">
+      <c r="G30" s="0">
         <v>955</v>
       </c>
     </row>
@@ -785,10 +941,13 @@
       <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="0">
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="0">
         <v>3420</v>
       </c>
-      <c r="F31" s="0">
+      <c r="G31" s="0">
         <v>1825</v>
       </c>
     </row>
@@ -805,10 +964,13 @@
       <c r="D32" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="0">
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="0">
         <v>2365</v>
       </c>
-      <c r="F32" s="0">
+      <c r="G32" s="0">
         <v>1400</v>
       </c>
     </row>
@@ -825,10 +987,13 @@
       <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="0">
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="0">
         <v>1440</v>
       </c>
-      <c r="F33" s="0">
+      <c r="G33" s="0">
         <v>775</v>
       </c>
     </row>
@@ -845,10 +1010,13 @@
       <c r="D34" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="0">
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="0">
         <v>1240</v>
       </c>
-      <c r="F34" s="0">
+      <c r="G34" s="0">
         <v>705</v>
       </c>
     </row>
@@ -865,10 +1033,13 @@
       <c r="D35" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="0">
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="0">
         <v>1940</v>
       </c>
-      <c r="F35" s="0">
+      <c r="G35" s="0">
         <v>1145</v>
       </c>
     </row>
@@ -885,10 +1056,13 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="0">
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="0">
         <v>2715</v>
       </c>
-      <c r="F36" s="0">
+      <c r="G36" s="0">
         <v>1585</v>
       </c>
     </row>
@@ -905,10 +1079,13 @@
       <c r="D37" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="0">
+      <c r="E37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="0">
         <v>2665</v>
       </c>
-      <c r="F37" s="0">
+      <c r="G37" s="0">
         <v>1565</v>
       </c>
     </row>
@@ -925,10 +1102,13 @@
       <c r="D38" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="0">
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="0">
         <v>1260</v>
       </c>
-      <c r="F38" s="0">
+      <c r="G38" s="0">
         <v>835</v>
       </c>
     </row>
@@ -945,10 +1125,13 @@
       <c r="D39" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="0">
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="0">
         <v>2235</v>
       </c>
-      <c r="F39" s="0">
+      <c r="G39" s="0">
         <v>1340</v>
       </c>
     </row>
@@ -965,10 +1148,13 @@
       <c r="D40" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="0">
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="0">
         <v>2480</v>
       </c>
-      <c r="F40" s="0">
+      <c r="G40" s="0">
         <v>1465</v>
       </c>
     </row>
@@ -985,12 +1171,15 @@
       <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="0">
-        <v>25</v>
+      <c r="E41" t="s">
+        <v>37</v>
       </c>
       <c r="F41" s="0">
         <v>25</v>
       </c>
+      <c r="G41" s="0">
+        <v>25</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
@@ -1005,10 +1194,13 @@
       <c r="D42" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="0">
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" s="0">
         <v>2480</v>
       </c>
-      <c r="F42" s="0">
+      <c r="G42" s="0">
         <v>1470</v>
       </c>
     </row>
@@ -1025,10 +1217,13 @@
       <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="0">
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" s="0">
         <v>185</v>
       </c>
-      <c r="F43" s="0">
+      <c r="G43" s="0">
         <v>155</v>
       </c>
     </row>
@@ -1045,10 +1240,13 @@
       <c r="D44" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="0">
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="0">
         <v>185</v>
       </c>
-      <c r="F44" s="0">
+      <c r="G44" s="0">
         <v>165</v>
       </c>
     </row>
@@ -1065,10 +1263,13 @@
       <c r="D45" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="0">
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="0">
         <v>115</v>
       </c>
-      <c r="F45" s="0">
+      <c r="G45" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1085,12 +1286,15 @@
       <c r="D46" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="0">
-        <v>40</v>
+      <c r="E46" t="s">
+        <v>41</v>
       </c>
       <c r="F46" s="0">
         <v>40</v>
       </c>
+      <c r="G46" s="0">
+        <v>40</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
@@ -1105,10 +1309,13 @@
       <c r="D47" t="s">
         <v>11</v>
       </c>
-      <c r="E47" s="0">
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="0">
         <v>2580</v>
       </c>
-      <c r="F47" s="0">
+      <c r="G47" s="0">
         <v>1540</v>
       </c>
     </row>
@@ -1125,10 +1332,13 @@
       <c r="D48" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="0">
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="0">
         <v>2585</v>
       </c>
-      <c r="F48" s="0">
+      <c r="G48" s="0">
         <v>1540</v>
       </c>
     </row>
@@ -1145,10 +1355,13 @@
       <c r="D49" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="0">
+      <c r="E49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="0">
         <v>270</v>
       </c>
-      <c r="F49" s="0">
+      <c r="G49" s="0">
         <v>230</v>
       </c>
     </row>
@@ -1165,10 +1378,13 @@
       <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="0">
+      <c r="E50" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="0">
         <v>260</v>
       </c>
-      <c r="F50" s="0">
+      <c r="G50" s="0">
         <v>215</v>
       </c>
     </row>
@@ -1185,10 +1401,13 @@
       <c r="D51" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="0">
+      <c r="E51" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="0">
         <v>315</v>
       </c>
-      <c r="F51" s="0">
+      <c r="G51" s="0">
         <v>260</v>
       </c>
     </row>
@@ -1205,10 +1424,13 @@
       <c r="D52" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="0">
+      <c r="E52" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52" s="0">
         <v>2490</v>
       </c>
-      <c r="F52" s="0">
+      <c r="G52" s="0">
         <v>1505</v>
       </c>
     </row>
@@ -1225,10 +1447,13 @@
       <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="0">
+      <c r="E53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="0">
         <v>1825</v>
       </c>
-      <c r="F53" s="0">
+      <c r="G53" s="0">
         <v>1235</v>
       </c>
     </row>
@@ -1245,10 +1470,13 @@
       <c r="D54" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="0">
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="0">
         <v>230</v>
       </c>
-      <c r="F54" s="0">
+      <c r="G54" s="0">
         <v>205</v>
       </c>
     </row>
@@ -1265,10 +1493,13 @@
       <c r="D55" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="0">
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="0">
         <v>2565</v>
       </c>
-      <c r="F55" s="0">
+      <c r="G55" s="0">
         <v>1530</v>
       </c>
     </row>
@@ -1285,10 +1516,13 @@
       <c r="D56" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="0">
+      <c r="E56" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="0">
         <v>380</v>
       </c>
-      <c r="F56" s="0">
+      <c r="G56" s="0">
         <v>310</v>
       </c>
     </row>
@@ -1305,10 +1539,13 @@
       <c r="D57" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="0">
+      <c r="E57" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="0">
         <v>2320</v>
       </c>
-      <c r="F57" s="0">
+      <c r="G57" s="0">
         <v>1420</v>
       </c>
     </row>
@@ -1325,10 +1562,13 @@
       <c r="D58" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="0">
+      <c r="E58" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" s="0">
         <v>370</v>
       </c>
-      <c r="F58" s="0">
+      <c r="G58" s="0">
         <v>305</v>
       </c>
     </row>
@@ -1345,10 +1585,13 @@
       <c r="D59" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="0">
+      <c r="E59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="0">
         <v>2550</v>
       </c>
-      <c r="F59" s="0">
+      <c r="G59" s="0">
         <v>1520</v>
       </c>
     </row>
@@ -1365,10 +1608,13 @@
       <c r="D60" t="s">
         <v>7</v>
       </c>
-      <c r="E60" s="0">
+      <c r="E60" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="0">
         <v>900</v>
       </c>
-      <c r="F60" s="0">
+      <c r="G60" s="0">
         <v>715</v>
       </c>
     </row>
@@ -1385,10 +1631,13 @@
       <c r="D61" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="0">
+      <c r="E61" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="0">
         <v>685</v>
       </c>
-      <c r="F61" s="0">
+      <c r="G61" s="0">
         <v>565</v>
       </c>
     </row>
@@ -1405,10 +1654,13 @@
       <c r="D62" t="s">
         <v>6</v>
       </c>
-      <c r="E62" s="0">
+      <c r="E62" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="0">
         <v>1450</v>
       </c>
-      <c r="F62" s="0">
+      <c r="G62" s="0">
         <v>1030</v>
       </c>
     </row>
@@ -1425,10 +1677,13 @@
       <c r="D63" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="0">
+      <c r="E63" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="0">
         <v>1085</v>
       </c>
-      <c r="F63" s="0">
+      <c r="G63" s="0">
         <v>820</v>
       </c>
     </row>
@@ -1445,10 +1700,13 @@
       <c r="D64" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="0">
+      <c r="E64" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" s="0">
         <v>750</v>
       </c>
-      <c r="F64" s="0">
+      <c r="G64" s="0">
         <v>595</v>
       </c>
     </row>
@@ -1465,10 +1723,13 @@
       <c r="D65" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="0">
+      <c r="E65" t="s">
+        <v>42</v>
+      </c>
+      <c r="F65" s="0">
         <v>75</v>
       </c>
-      <c r="F65" s="0">
+      <c r="G65" s="0">
         <v>60</v>
       </c>
     </row>
@@ -1485,10 +1746,13 @@
       <c r="D66" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="0">
+      <c r="E66" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="0">
         <v>550</v>
       </c>
-      <c r="F66" s="0">
+      <c r="G66" s="0">
         <v>455</v>
       </c>
     </row>
@@ -1505,10 +1769,13 @@
       <c r="D67" t="s">
         <v>7</v>
       </c>
-      <c r="E67" s="0">
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="0">
         <v>535</v>
       </c>
-      <c r="F67" s="0">
+      <c r="G67" s="0">
         <v>450</v>
       </c>
     </row>
@@ -1525,10 +1792,13 @@
       <c r="D68" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="0">
+      <c r="E68" t="s">
+        <v>43</v>
+      </c>
+      <c r="F68" s="0">
         <v>530</v>
       </c>
-      <c r="F68" s="0">
+      <c r="G68" s="0">
         <v>445</v>
       </c>
     </row>
@@ -1545,10 +1815,13 @@
       <c r="D69" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="0">
+      <c r="E69" t="s">
+        <v>44</v>
+      </c>
+      <c r="F69" s="0">
         <v>1370</v>
       </c>
-      <c r="F69" s="0">
+      <c r="G69" s="0">
         <v>750</v>
       </c>
     </row>
@@ -1565,10 +1838,13 @@
       <c r="D70" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="0">
+      <c r="E70" t="s">
+        <v>44</v>
+      </c>
+      <c r="F70" s="0">
         <v>1685</v>
       </c>
-      <c r="F70" s="0">
+      <c r="G70" s="0">
         <v>950</v>
       </c>
     </row>
@@ -1585,10 +1861,13 @@
       <c r="D71" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="0">
+      <c r="E71" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" s="0">
         <v>90</v>
       </c>
-      <c r="F71" s="0">
+      <c r="G71" s="0">
         <v>80</v>
       </c>
     </row>
@@ -1605,10 +1884,13 @@
       <c r="D72" t="s">
         <v>12</v>
       </c>
-      <c r="E72" s="0">
+      <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" s="0">
         <v>1695</v>
       </c>
-      <c r="F72" s="0">
+      <c r="G72" s="0">
         <v>950</v>
       </c>
     </row>
@@ -1625,10 +1907,13 @@
       <c r="D73" t="s">
         <v>13</v>
       </c>
-      <c r="E73" s="0">
+      <c r="E73" t="s">
+        <v>37</v>
+      </c>
+      <c r="F73" s="0">
         <v>1905</v>
       </c>
-      <c r="F73" s="0">
+      <c r="G73" s="0">
         <v>1105</v>
       </c>
     </row>
@@ -1645,10 +1930,13 @@
       <c r="D74" t="s">
         <v>13</v>
       </c>
-      <c r="E74" s="0">
+      <c r="E74" t="s">
+        <v>37</v>
+      </c>
+      <c r="F74" s="0">
         <v>1890</v>
       </c>
-      <c r="F74" s="0">
+      <c r="G74" s="0">
         <v>1110</v>
       </c>
     </row>
@@ -1665,10 +1953,13 @@
       <c r="D75" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="0">
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" s="0">
         <v>455</v>
       </c>
-      <c r="F75" s="0">
+      <c r="G75" s="0">
         <v>390</v>
       </c>
     </row>
@@ -1685,10 +1976,13 @@
       <c r="D76" t="s">
         <v>7</v>
       </c>
-      <c r="E76" s="0">
+      <c r="E76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="0">
         <v>460</v>
       </c>
-      <c r="F76" s="0">
+      <c r="G76" s="0">
         <v>400</v>
       </c>
     </row>
@@ -1705,10 +1999,13 @@
       <c r="D77" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="0">
+      <c r="E77" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="0">
         <v>445</v>
       </c>
-      <c r="F77" s="0">
+      <c r="G77" s="0">
         <v>390</v>
       </c>
     </row>
@@ -1725,10 +2022,13 @@
       <c r="D78" t="s">
         <v>14</v>
       </c>
-      <c r="E78" s="0">
+      <c r="E78" t="s">
+        <v>37</v>
+      </c>
+      <c r="F78" s="0">
         <v>115</v>
       </c>
-      <c r="F78" s="0">
+      <c r="G78" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1745,10 +2045,13 @@
       <c r="D79" t="s">
         <v>14</v>
       </c>
-      <c r="E79" s="0">
+      <c r="E79" t="s">
+        <v>37</v>
+      </c>
+      <c r="F79" s="0">
         <v>165</v>
       </c>
-      <c r="F79" s="0">
+      <c r="G79" s="0">
         <v>155</v>
       </c>
     </row>
@@ -1765,10 +2068,13 @@
       <c r="D80" t="s">
         <v>13</v>
       </c>
-      <c r="E80" s="0">
+      <c r="E80" t="s">
+        <v>37</v>
+      </c>
+      <c r="F80" s="0">
         <v>1670</v>
       </c>
-      <c r="F80" s="0">
+      <c r="G80" s="0">
         <v>1035</v>
       </c>
     </row>
@@ -1785,10 +2091,13 @@
       <c r="D81" t="s">
         <v>13</v>
       </c>
-      <c r="E81" s="0">
+      <c r="E81" t="s">
+        <v>37</v>
+      </c>
+      <c r="F81" s="0">
         <v>815</v>
       </c>
-      <c r="F81" s="0">
+      <c r="G81" s="0">
         <v>590</v>
       </c>
     </row>
@@ -1805,10 +2114,13 @@
       <c r="D82" t="s">
         <v>13</v>
       </c>
-      <c r="E82" s="0">
+      <c r="E82" t="s">
+        <v>37</v>
+      </c>
+      <c r="F82" s="0">
         <v>280</v>
       </c>
-      <c r="F82" s="0">
+      <c r="G82" s="0">
         <v>225</v>
       </c>
     </row>
@@ -1825,10 +2137,13 @@
       <c r="D83" t="s">
         <v>6</v>
       </c>
-      <c r="E83" s="0">
+      <c r="E83" t="s">
+        <v>46</v>
+      </c>
+      <c r="F83" s="0">
         <v>190</v>
       </c>
-      <c r="F83" s="0">
+      <c r="G83" s="0">
         <v>160</v>
       </c>
     </row>
@@ -1845,10 +2160,13 @@
       <c r="D84" t="s">
         <v>13</v>
       </c>
-      <c r="E84" s="0">
+      <c r="E84" t="s">
+        <v>37</v>
+      </c>
+      <c r="F84" s="0">
         <v>625</v>
       </c>
-      <c r="F84" s="0">
+      <c r="G84" s="0">
         <v>465</v>
       </c>
     </row>
@@ -1865,12 +2183,15 @@
       <c r="D85" t="s">
         <v>6</v>
       </c>
-      <c r="E85" s="0">
-        <v>10</v>
+      <c r="E85" t="s">
+        <v>47</v>
       </c>
       <c r="F85" s="0">
         <v>10</v>
       </c>
+      <c r="G85" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
@@ -1885,12 +2206,15 @@
       <c r="D86" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="0">
-        <v>30</v>
+      <c r="E86" t="s">
+        <v>47</v>
       </c>
       <c r="F86" s="0">
         <v>30</v>
       </c>
+      <c r="G86" s="0">
+        <v>30</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
@@ -1905,10 +2229,13 @@
       <c r="D87" t="s">
         <v>7</v>
       </c>
-      <c r="E87" s="0">
+      <c r="E87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="0">
         <v>460</v>
       </c>
-      <c r="F87" s="0">
+      <c r="G87" s="0">
         <v>400</v>
       </c>
     </row>
@@ -1925,10 +2252,13 @@
       <c r="D88" t="s">
         <v>7</v>
       </c>
-      <c r="E88" s="0">
+      <c r="E88" t="s">
+        <v>45</v>
+      </c>
+      <c r="F88" s="0">
         <v>395</v>
       </c>
-      <c r="F88" s="0">
+      <c r="G88" s="0">
         <v>360</v>
       </c>
     </row>
@@ -1945,10 +2275,13 @@
       <c r="D89" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="0">
+      <c r="E89" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" s="0">
         <v>400</v>
       </c>
-      <c r="F89" s="0">
+      <c r="G89" s="0">
         <v>360</v>
       </c>
     </row>
@@ -1965,10 +2298,13 @@
       <c r="D90" t="s">
         <v>7</v>
       </c>
-      <c r="E90" s="0">
+      <c r="E90" t="s">
+        <v>45</v>
+      </c>
+      <c r="F90" s="0">
         <v>365</v>
       </c>
-      <c r="F90" s="0">
+      <c r="G90" s="0">
         <v>335</v>
       </c>
     </row>
@@ -1985,10 +2321,13 @@
       <c r="D91" t="s">
         <v>15</v>
       </c>
-      <c r="E91" s="0">
+      <c r="E91" t="s">
+        <v>37</v>
+      </c>
+      <c r="F91" s="0">
         <v>255</v>
       </c>
-      <c r="F91" s="0">
+      <c r="G91" s="0">
         <v>230</v>
       </c>
     </row>
@@ -2005,10 +2344,13 @@
       <c r="D92" t="s">
         <v>15</v>
       </c>
-      <c r="E92" s="0">
+      <c r="E92" t="s">
+        <v>37</v>
+      </c>
+      <c r="F92" s="0">
         <v>70</v>
       </c>
-      <c r="F92" s="0">
+      <c r="G92" s="0">
         <v>65</v>
       </c>
     </row>
@@ -2025,10 +2367,13 @@
       <c r="D93" t="s">
         <v>14</v>
       </c>
-      <c r="E93" s="0">
+      <c r="E93" t="s">
+        <v>37</v>
+      </c>
+      <c r="F93" s="0">
         <v>245</v>
       </c>
-      <c r="F93" s="0">
+      <c r="G93" s="0">
         <v>220</v>
       </c>
     </row>
@@ -2045,12 +2390,15 @@
       <c r="D94" t="s">
         <v>15</v>
       </c>
-      <c r="E94" s="0">
-        <v>10</v>
+      <c r="E94" t="s">
+        <v>37</v>
       </c>
       <c r="F94" s="0">
         <v>10</v>
       </c>
+      <c r="G94" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
@@ -2065,10 +2413,13 @@
       <c r="D95" t="s">
         <v>7</v>
       </c>
-      <c r="E95" s="0">
+      <c r="E95" t="s">
+        <v>45</v>
+      </c>
+      <c r="F95" s="0">
         <v>360</v>
       </c>
-      <c r="F95" s="0">
+      <c r="G95" s="0">
         <v>335</v>
       </c>
     </row>
@@ -2085,10 +2436,13 @@
       <c r="D96" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="0">
+      <c r="E96" t="s">
+        <v>48</v>
+      </c>
+      <c r="F96" s="0">
         <v>395</v>
       </c>
-      <c r="F96" s="0">
+      <c r="G96" s="0">
         <v>360</v>
       </c>
     </row>
@@ -2105,10 +2459,13 @@
       <c r="D97" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="0">
+      <c r="E97" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" s="0">
         <v>385</v>
       </c>
-      <c r="F97" s="0">
+      <c r="G97" s="0">
         <v>360</v>
       </c>
     </row>
@@ -2125,12 +2482,15 @@
       <c r="D98" t="s">
         <v>6</v>
       </c>
-      <c r="E98" s="0">
-        <v>55</v>
+      <c r="E98" t="s">
+        <v>49</v>
       </c>
       <c r="F98" s="0">
         <v>55</v>
       </c>
+      <c r="G98" s="0">
+        <v>55</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
@@ -2145,10 +2505,13 @@
       <c r="D99" t="s">
         <v>6</v>
       </c>
-      <c r="E99" s="0">
+      <c r="E99" t="s">
+        <v>49</v>
+      </c>
+      <c r="F99" s="0">
         <v>50</v>
       </c>
-      <c r="F99" s="0">
+      <c r="G99" s="0">
         <v>45</v>
       </c>
     </row>
@@ -2165,12 +2528,15 @@
       <c r="D100" t="s">
         <v>6</v>
       </c>
-      <c r="E100" s="0">
-        <v>5</v>
+      <c r="E100" t="s">
+        <v>49</v>
       </c>
       <c r="F100" s="0">
         <v>5</v>
       </c>
+      <c r="G100" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
@@ -2185,10 +2551,13 @@
       <c r="D101" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="0">
+      <c r="E101" t="s">
+        <v>50</v>
+      </c>
+      <c r="F101" s="0">
         <v>355</v>
       </c>
-      <c r="F101" s="0">
+      <c r="G101" s="0">
         <v>330</v>
       </c>
     </row>
@@ -2205,10 +2574,13 @@
       <c r="D102" t="s">
         <v>7</v>
       </c>
-      <c r="E102" s="0">
+      <c r="E102" t="s">
+        <v>48</v>
+      </c>
+      <c r="F102" s="0">
         <v>390</v>
       </c>
-      <c r="F102" s="0">
+      <c r="G102" s="0">
         <v>360</v>
       </c>
     </row>
@@ -2225,10 +2597,13 @@
       <c r="D103" t="s">
         <v>7</v>
       </c>
-      <c r="E103" s="0">
+      <c r="E103" t="s">
+        <v>48</v>
+      </c>
+      <c r="F103" s="0">
         <v>440</v>
       </c>
-      <c r="F103" s="0">
+      <c r="G103" s="0">
         <v>395</v>
       </c>
     </row>
@@ -2245,10 +2620,13 @@
       <c r="D104" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="0">
+      <c r="E104" t="s">
+        <v>48</v>
+      </c>
+      <c r="F104" s="0">
         <v>410</v>
       </c>
-      <c r="F104" s="0">
+      <c r="G104" s="0">
         <v>380</v>
       </c>
     </row>
@@ -2265,12 +2643,15 @@
       <c r="D105" t="s">
         <v>6</v>
       </c>
-      <c r="E105" s="0">
-        <v>20</v>
+      <c r="E105" t="s">
+        <v>49</v>
       </c>
       <c r="F105" s="0">
         <v>20</v>
       </c>
+      <c r="G105" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
@@ -2285,10 +2666,13 @@
       <c r="D106" t="s">
         <v>6</v>
       </c>
-      <c r="E106" s="0">
+      <c r="E106" t="s">
+        <v>49</v>
+      </c>
+      <c r="F106" s="0">
         <v>85</v>
       </c>
-      <c r="F106" s="0">
+      <c r="G106" s="0">
         <v>80</v>
       </c>
     </row>
@@ -2305,12 +2689,15 @@
       <c r="D107" t="s">
         <v>16</v>
       </c>
-      <c r="E107" s="0">
-        <v>65</v>
+      <c r="E107" t="s">
+        <v>37</v>
       </c>
       <c r="F107" s="0">
         <v>65</v>
       </c>
+      <c r="G107" s="0">
+        <v>65</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
@@ -2325,10 +2712,13 @@
       <c r="D108" t="s">
         <v>6</v>
       </c>
-      <c r="E108" s="0">
+      <c r="E108" t="s">
+        <v>49</v>
+      </c>
+      <c r="F108" s="0">
         <v>440</v>
       </c>
-      <c r="F108" s="0">
+      <c r="G108" s="0">
         <v>395</v>
       </c>
     </row>
@@ -2345,10 +2735,13 @@
       <c r="D109" t="s">
         <v>17</v>
       </c>
-      <c r="E109" s="0">
+      <c r="E109" t="s">
+        <v>37</v>
+      </c>
+      <c r="F109" s="0">
         <v>430</v>
       </c>
-      <c r="F109" s="0">
+      <c r="G109" s="0">
         <v>410</v>
       </c>
     </row>
@@ -2365,10 +2758,13 @@
       <c r="D110" t="s">
         <v>7</v>
       </c>
-      <c r="E110" s="0">
+      <c r="E110" t="s">
+        <v>50</v>
+      </c>
+      <c r="F110" s="0">
         <v>365</v>
       </c>
-      <c r="F110" s="0">
+      <c r="G110" s="0">
         <v>335</v>
       </c>
     </row>
@@ -2385,10 +2781,13 @@
       <c r="D111" t="s">
         <v>17</v>
       </c>
-      <c r="E111" s="0">
+      <c r="E111" t="s">
+        <v>37</v>
+      </c>
+      <c r="F111" s="0">
         <v>390</v>
       </c>
-      <c r="F111" s="0">
+      <c r="G111" s="0">
         <v>375</v>
       </c>
     </row>
@@ -2405,10 +2804,13 @@
       <c r="D112" t="s">
         <v>16</v>
       </c>
-      <c r="E112" s="0">
+      <c r="E112" t="s">
+        <v>37</v>
+      </c>
+      <c r="F112" s="0">
         <v>70</v>
       </c>
-      <c r="F112" s="0">
+      <c r="G112" s="0">
         <v>65</v>
       </c>
     </row>
@@ -2425,12 +2827,15 @@
       <c r="D113" t="s">
         <v>16</v>
       </c>
-      <c r="E113" s="0">
-        <v>70</v>
+      <c r="E113" t="s">
+        <v>37</v>
       </c>
       <c r="F113" s="0">
         <v>70</v>
       </c>
+      <c r="G113" s="0">
+        <v>70</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
@@ -2445,10 +2850,13 @@
       <c r="D114" t="s">
         <v>7</v>
       </c>
-      <c r="E114" s="0">
+      <c r="E114" t="s">
+        <v>50</v>
+      </c>
+      <c r="F114" s="0">
         <v>360</v>
       </c>
-      <c r="F114" s="0">
+      <c r="G114" s="0">
         <v>335</v>
       </c>
     </row>
@@ -2465,10 +2873,13 @@
       <c r="D115" t="s">
         <v>18</v>
       </c>
-      <c r="E115" s="0">
+      <c r="E115" t="s">
+        <v>37</v>
+      </c>
+      <c r="F115" s="0">
         <v>65</v>
       </c>
-      <c r="F115" s="0">
+      <c r="G115" s="0">
         <v>55</v>
       </c>
     </row>
@@ -2485,10 +2896,13 @@
       <c r="D116" t="s">
         <v>18</v>
       </c>
-      <c r="E116" s="0">
+      <c r="E116" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" s="0">
         <v>110</v>
       </c>
-      <c r="F116" s="0">
+      <c r="G116" s="0">
         <v>95</v>
       </c>
     </row>
@@ -2505,10 +2919,13 @@
       <c r="D117" t="s">
         <v>17</v>
       </c>
-      <c r="E117" s="0">
+      <c r="E117" t="s">
+        <v>37</v>
+      </c>
+      <c r="F117" s="0">
         <v>395</v>
       </c>
-      <c r="F117" s="0">
+      <c r="G117" s="0">
         <v>370</v>
       </c>
     </row>
@@ -2525,10 +2942,13 @@
       <c r="D118" t="s">
         <v>17</v>
       </c>
-      <c r="E118" s="0">
+      <c r="E118" t="s">
+        <v>37</v>
+      </c>
+      <c r="F118" s="0">
         <v>385</v>
       </c>
-      <c r="F118" s="0">
+      <c r="G118" s="0">
         <v>360</v>
       </c>
     </row>
@@ -2545,10 +2965,13 @@
       <c r="D119" t="s">
         <v>18</v>
       </c>
-      <c r="E119" s="0">
+      <c r="E119" t="s">
+        <v>37</v>
+      </c>
+      <c r="F119" s="0">
         <v>105</v>
       </c>
-      <c r="F119" s="0">
+      <c r="G119" s="0">
         <v>90</v>
       </c>
     </row>
@@ -2565,10 +2988,13 @@
       <c r="D120" t="s">
         <v>7</v>
       </c>
-      <c r="E120" s="0">
+      <c r="E120" t="s">
+        <v>48</v>
+      </c>
+      <c r="F120" s="0">
         <v>280</v>
       </c>
-      <c r="F120" s="0">
+      <c r="G120" s="0">
         <v>260</v>
       </c>
     </row>
@@ -2585,10 +3011,13 @@
       <c r="D121" t="s">
         <v>7</v>
       </c>
-      <c r="E121" s="0">
+      <c r="E121" t="s">
+        <v>48</v>
+      </c>
+      <c r="F121" s="0">
         <v>395</v>
       </c>
-      <c r="F121" s="0">
+      <c r="G121" s="0">
         <v>360</v>
       </c>
     </row>
@@ -2605,12 +3034,15 @@
       <c r="D122" t="s">
         <v>16</v>
       </c>
-      <c r="E122" s="0">
-        <v>70</v>
+      <c r="E122" t="s">
+        <v>37</v>
       </c>
       <c r="F122" s="0">
         <v>70</v>
       </c>
+      <c r="G122" s="0">
+        <v>70</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
@@ -2625,10 +3057,13 @@
       <c r="D123" t="s">
         <v>16</v>
       </c>
-      <c r="E123" s="0">
+      <c r="E123" t="s">
+        <v>37</v>
+      </c>
+      <c r="F123" s="0">
         <v>75</v>
       </c>
-      <c r="F123" s="0">
+      <c r="G123" s="0">
         <v>70</v>
       </c>
     </row>
@@ -2645,12 +3080,15 @@
       <c r="D124" t="s">
         <v>16</v>
       </c>
-      <c r="E124" s="0">
-        <v>80</v>
+      <c r="E124" t="s">
+        <v>37</v>
       </c>
       <c r="F124" s="0">
         <v>80</v>
       </c>
+      <c r="G124" s="0">
+        <v>80</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
@@ -2665,10 +3103,13 @@
       <c r="D125" t="s">
         <v>19</v>
       </c>
-      <c r="E125" s="0">
+      <c r="E125" t="s">
+        <v>37</v>
+      </c>
+      <c r="F125" s="0">
         <v>95</v>
       </c>
-      <c r="F125" s="0">
+      <c r="G125" s="0">
         <v>90</v>
       </c>
     </row>
@@ -2685,10 +3126,13 @@
       <c r="D126" t="s">
         <v>19</v>
       </c>
-      <c r="E126" s="0">
+      <c r="E126" t="s">
+        <v>37</v>
+      </c>
+      <c r="F126" s="0">
         <v>90</v>
       </c>
-      <c r="F126" s="0">
+      <c r="G126" s="0">
         <v>85</v>
       </c>
     </row>
@@ -2705,12 +3149,15 @@
       <c r="D127" t="s">
         <v>20</v>
       </c>
-      <c r="E127" s="0">
-        <v>10</v>
+      <c r="E127" t="s">
+        <v>37</v>
       </c>
       <c r="F127" s="0">
         <v>10</v>
       </c>
+      <c r="G127" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
@@ -2725,12 +3172,15 @@
       <c r="D128" t="s">
         <v>20</v>
       </c>
-      <c r="E128" s="0">
-        <v>20</v>
+      <c r="E128" t="s">
+        <v>37</v>
       </c>
       <c r="F128" s="0">
         <v>20</v>
       </c>
+      <c r="G128" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
@@ -2745,10 +3195,13 @@
       <c r="D129" t="s">
         <v>15</v>
       </c>
-      <c r="E129" s="0">
+      <c r="E129" t="s">
+        <v>37</v>
+      </c>
+      <c r="F129" s="0">
         <v>235</v>
       </c>
-      <c r="F129" s="0">
+      <c r="G129" s="0">
         <v>195</v>
       </c>
     </row>
@@ -2765,12 +3218,15 @@
       <c r="D130" t="s">
         <v>20</v>
       </c>
-      <c r="E130" s="0">
-        <v>15</v>
+      <c r="E130" t="s">
+        <v>37</v>
       </c>
       <c r="F130" s="0">
         <v>15</v>
       </c>
+      <c r="G130" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
@@ -2785,10 +3241,13 @@
       <c r="D131" t="s">
         <v>14</v>
       </c>
-      <c r="E131" s="0">
+      <c r="E131" t="s">
+        <v>37</v>
+      </c>
+      <c r="F131" s="0">
         <v>210</v>
       </c>
-      <c r="F131" s="0">
+      <c r="G131" s="0">
         <v>175</v>
       </c>
     </row>
@@ -2805,10 +3264,13 @@
       <c r="D132" t="s">
         <v>14</v>
       </c>
-      <c r="E132" s="0">
+      <c r="E132" t="s">
+        <v>37</v>
+      </c>
+      <c r="F132" s="0">
         <v>300</v>
       </c>
-      <c r="F132" s="0">
+      <c r="G132" s="0">
         <v>235</v>
       </c>
     </row>
@@ -2825,10 +3287,13 @@
       <c r="D133" t="s">
         <v>14</v>
       </c>
-      <c r="E133" s="0">
+      <c r="E133" t="s">
+        <v>37</v>
+      </c>
+      <c r="F133" s="0">
         <v>290</v>
       </c>
-      <c r="F133" s="0">
+      <c r="G133" s="0">
         <v>240</v>
       </c>
     </row>
@@ -2845,10 +3310,13 @@
       <c r="D134" t="s">
         <v>20</v>
       </c>
-      <c r="E134" s="0">
+      <c r="E134" t="s">
+        <v>37</v>
+      </c>
+      <c r="F134" s="0">
         <v>25</v>
       </c>
-      <c r="F134" s="0">
+      <c r="G134" s="0">
         <v>20</v>
       </c>
     </row>
@@ -2865,10 +3333,13 @@
       <c r="D135" t="s">
         <v>14</v>
       </c>
-      <c r="E135" s="0">
+      <c r="E135" t="s">
+        <v>37</v>
+      </c>
+      <c r="F135" s="0">
         <v>25</v>
       </c>
-      <c r="F135" s="0">
+      <c r="G135" s="0">
         <v>20</v>
       </c>
     </row>
@@ -2885,10 +3356,13 @@
       <c r="D136" t="s">
         <v>14</v>
       </c>
-      <c r="E136" s="0">
+      <c r="E136" t="s">
+        <v>37</v>
+      </c>
+      <c r="F136" s="0">
         <v>380</v>
       </c>
-      <c r="F136" s="0">
+      <c r="G136" s="0">
         <v>310</v>
       </c>
     </row>
@@ -2905,10 +3379,13 @@
       <c r="D137" t="s">
         <v>14</v>
       </c>
-      <c r="E137" s="0">
+      <c r="E137" t="s">
+        <v>37</v>
+      </c>
+      <c r="F137" s="0">
         <v>540</v>
       </c>
-      <c r="F137" s="0">
+      <c r="G137" s="0">
         <v>345</v>
       </c>
     </row>
@@ -2925,10 +3402,13 @@
       <c r="D138" t="s">
         <v>14</v>
       </c>
-      <c r="E138" s="0">
+      <c r="E138" t="s">
+        <v>37</v>
+      </c>
+      <c r="F138" s="0">
         <v>440</v>
       </c>
-      <c r="F138" s="0">
+      <c r="G138" s="0">
         <v>340</v>
       </c>
     </row>
@@ -2945,10 +3425,13 @@
       <c r="D139" t="s">
         <v>14</v>
       </c>
-      <c r="E139" s="0">
+      <c r="E139" t="s">
+        <v>37</v>
+      </c>
+      <c r="F139" s="0">
         <v>235</v>
       </c>
-      <c r="F139" s="0">
+      <c r="G139" s="0">
         <v>215</v>
       </c>
     </row>
@@ -2965,10 +3448,13 @@
       <c r="D140" t="s">
         <v>14</v>
       </c>
-      <c r="E140" s="0">
+      <c r="E140" t="s">
+        <v>37</v>
+      </c>
+      <c r="F140" s="0">
         <v>120</v>
       </c>
-      <c r="F140" s="0">
+      <c r="G140" s="0">
         <v>110</v>
       </c>
     </row>
@@ -2985,10 +3471,13 @@
       <c r="D141" t="s">
         <v>14</v>
       </c>
-      <c r="E141" s="0">
+      <c r="E141" t="s">
+        <v>37</v>
+      </c>
+      <c r="F141" s="0">
         <v>385</v>
       </c>
-      <c r="F141" s="0">
+      <c r="G141" s="0">
         <v>315</v>
       </c>
     </row>
@@ -3005,10 +3494,13 @@
       <c r="D142" t="s">
         <v>14</v>
       </c>
-      <c r="E142" s="0">
+      <c r="E142" t="s">
+        <v>37</v>
+      </c>
+      <c r="F142" s="0">
         <v>555</v>
       </c>
-      <c r="F142" s="0">
+      <c r="G142" s="0">
         <v>410</v>
       </c>
     </row>
@@ -3025,10 +3517,13 @@
       <c r="D143" t="s">
         <v>14</v>
       </c>
-      <c r="E143" s="0">
+      <c r="E143" t="s">
+        <v>37</v>
+      </c>
+      <c r="F143" s="0">
         <v>145</v>
       </c>
-      <c r="F143" s="0">
+      <c r="G143" s="0">
         <v>95</v>
       </c>
     </row>
@@ -3045,10 +3540,13 @@
       <c r="D144" t="s">
         <v>19</v>
       </c>
-      <c r="E144" s="0">
+      <c r="E144" t="s">
+        <v>37</v>
+      </c>
+      <c r="F144" s="0">
         <v>105</v>
       </c>
-      <c r="F144" s="0">
+      <c r="G144" s="0">
         <v>95</v>
       </c>
     </row>
@@ -3065,10 +3563,13 @@
       <c r="D145" t="s">
         <v>21</v>
       </c>
-      <c r="E145" s="0">
+      <c r="E145" t="s">
+        <v>37</v>
+      </c>
+      <c r="F145" s="0">
         <v>895</v>
       </c>
-      <c r="F145" s="0">
+      <c r="G145" s="0">
         <v>525</v>
       </c>
     </row>
@@ -3085,10 +3586,13 @@
       <c r="D146" t="s">
         <v>21</v>
       </c>
-      <c r="E146" s="0">
+      <c r="E146" t="s">
+        <v>37</v>
+      </c>
+      <c r="F146" s="0">
         <v>430</v>
       </c>
-      <c r="F146" s="0">
+      <c r="G146" s="0">
         <v>310</v>
       </c>
     </row>
@@ -3105,10 +3609,13 @@
       <c r="D147" t="s">
         <v>21</v>
       </c>
-      <c r="E147" s="0">
+      <c r="E147" t="s">
+        <v>37</v>
+      </c>
+      <c r="F147" s="0">
         <v>655</v>
       </c>
-      <c r="F147" s="0">
+      <c r="G147" s="0">
         <v>430</v>
       </c>
     </row>
@@ -3125,10 +3632,13 @@
       <c r="D148" t="s">
         <v>12</v>
       </c>
-      <c r="E148" s="0">
+      <c r="E148" t="s">
+        <v>44</v>
+      </c>
+      <c r="F148" s="0">
         <v>2320</v>
       </c>
-      <c r="F148" s="0">
+      <c r="G148" s="0">
         <v>1275</v>
       </c>
     </row>
@@ -3145,10 +3655,13 @@
       <c r="D149" t="s">
         <v>12</v>
       </c>
-      <c r="E149" s="0">
+      <c r="E149" t="s">
+        <v>44</v>
+      </c>
+      <c r="F149" s="0">
         <v>1960</v>
       </c>
-      <c r="F149" s="0">
+      <c r="G149" s="0">
         <v>1115</v>
       </c>
     </row>
@@ -3165,12 +3678,15 @@
       <c r="D150" t="s">
         <v>22</v>
       </c>
-      <c r="E150" s="0">
-        <v>45</v>
+      <c r="E150" t="s">
+        <v>51</v>
       </c>
       <c r="F150" s="0">
         <v>45</v>
       </c>
+      <c r="G150" s="0">
+        <v>45</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
@@ -3185,10 +3701,13 @@
       <c r="D151" t="s">
         <v>21</v>
       </c>
-      <c r="E151" s="0">
+      <c r="E151" t="s">
+        <v>37</v>
+      </c>
+      <c r="F151" s="0">
         <v>545</v>
       </c>
-      <c r="F151" s="0">
+      <c r="G151" s="0">
         <v>360</v>
       </c>
     </row>
@@ -3205,10 +3724,13 @@
       <c r="D152" t="s">
         <v>22</v>
       </c>
-      <c r="E152" s="0">
+      <c r="E152" t="s">
+        <v>52</v>
+      </c>
+      <c r="F152" s="0">
         <v>185</v>
       </c>
-      <c r="F152" s="0">
+      <c r="G152" s="0">
         <v>150</v>
       </c>
     </row>
@@ -3225,10 +3747,13 @@
       <c r="D153" t="s">
         <v>22</v>
       </c>
-      <c r="E153" s="0">
+      <c r="E153" t="s">
+        <v>52</v>
+      </c>
+      <c r="F153" s="0">
         <v>100</v>
       </c>
-      <c r="F153" s="0">
+      <c r="G153" s="0">
         <v>85</v>
       </c>
     </row>
@@ -3245,10 +3770,13 @@
       <c r="D154" t="s">
         <v>22</v>
       </c>
-      <c r="E154" s="0">
+      <c r="E154" t="s">
+        <v>52</v>
+      </c>
+      <c r="F154" s="0">
         <v>25</v>
       </c>
-      <c r="F154" s="0">
+      <c r="G154" s="0">
         <v>20</v>
       </c>
     </row>
@@ -3265,10 +3793,13 @@
       <c r="D155" t="s">
         <v>22</v>
       </c>
-      <c r="E155" s="0">
+      <c r="E155" t="s">
+        <v>52</v>
+      </c>
+      <c r="F155" s="0">
         <v>300</v>
       </c>
-      <c r="F155" s="0">
+      <c r="G155" s="0">
         <v>240</v>
       </c>
     </row>
@@ -3285,10 +3816,13 @@
       <c r="D156" t="s">
         <v>22</v>
       </c>
-      <c r="E156" s="0">
+      <c r="E156" t="s">
+        <v>52</v>
+      </c>
+      <c r="F156" s="0">
         <v>395</v>
       </c>
-      <c r="F156" s="0">
+      <c r="G156" s="0">
         <v>325</v>
       </c>
     </row>
@@ -3305,10 +3839,13 @@
       <c r="D157" t="s">
         <v>22</v>
       </c>
-      <c r="E157" s="0">
+      <c r="E157" t="s">
+        <v>52</v>
+      </c>
+      <c r="F157" s="0">
         <v>465</v>
       </c>
-      <c r="F157" s="0">
+      <c r="G157" s="0">
         <v>380</v>
       </c>
     </row>
@@ -3325,10 +3862,13 @@
       <c r="D158" t="s">
         <v>22</v>
       </c>
-      <c r="E158" s="0">
+      <c r="E158" t="s">
+        <v>52</v>
+      </c>
+      <c r="F158" s="0">
         <v>410</v>
       </c>
-      <c r="F158" s="0">
+      <c r="G158" s="0">
         <v>345</v>
       </c>
     </row>
@@ -3345,10 +3885,13 @@
       <c r="D159" t="s">
         <v>22</v>
       </c>
-      <c r="E159" s="0">
+      <c r="E159" t="s">
+        <v>52</v>
+      </c>
+      <c r="F159" s="0">
         <v>470</v>
       </c>
-      <c r="F159" s="0">
+      <c r="G159" s="0">
         <v>385</v>
       </c>
     </row>
@@ -3365,12 +3908,15 @@
       <c r="D160" t="s">
         <v>23</v>
       </c>
-      <c r="E160" s="0">
-        <v>20</v>
+      <c r="E160" t="s">
+        <v>37</v>
       </c>
       <c r="F160" s="0">
         <v>20</v>
       </c>
+      <c r="G160" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
@@ -3385,12 +3931,15 @@
       <c r="D161" t="s">
         <v>23</v>
       </c>
-      <c r="E161" s="0">
-        <v>10</v>
+      <c r="E161" t="s">
+        <v>37</v>
       </c>
       <c r="F161" s="0">
         <v>10</v>
       </c>
+      <c r="G161" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
@@ -3405,12 +3954,15 @@
       <c r="D162" t="s">
         <v>23</v>
       </c>
-      <c r="E162" s="0">
-        <v>20</v>
+      <c r="E162" t="s">
+        <v>37</v>
       </c>
       <c r="F162" s="0">
         <v>20</v>
       </c>
+      <c r="G162" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
@@ -3425,12 +3977,15 @@
       <c r="D163" t="s">
         <v>23</v>
       </c>
-      <c r="E163" s="0">
-        <v>5</v>
+      <c r="E163" t="s">
+        <v>37</v>
       </c>
       <c r="F163" s="0">
         <v>5</v>
       </c>
+      <c r="G163" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
@@ -3445,10 +4000,13 @@
       <c r="D164" t="s">
         <v>23</v>
       </c>
-      <c r="E164" s="0">
+      <c r="E164" t="s">
+        <v>37</v>
+      </c>
+      <c r="F164" s="0">
         <v>20</v>
       </c>
-      <c r="F164" s="0">
+      <c r="G164" s="0">
         <v>15</v>
       </c>
     </row>
@@ -3465,10 +4023,13 @@
       <c r="D165" t="s">
         <v>22</v>
       </c>
-      <c r="E165" s="0">
+      <c r="E165" t="s">
+        <v>52</v>
+      </c>
+      <c r="F165" s="0">
         <v>250</v>
       </c>
-      <c r="F165" s="0">
+      <c r="G165" s="0">
         <v>205</v>
       </c>
     </row>
@@ -3485,10 +4046,13 @@
       <c r="D166" t="s">
         <v>22</v>
       </c>
-      <c r="E166" s="0">
+      <c r="E166" t="s">
+        <v>51</v>
+      </c>
+      <c r="F166" s="0">
         <v>165</v>
       </c>
-      <c r="F166" s="0">
+      <c r="G166" s="0">
         <v>135</v>
       </c>
     </row>
@@ -3505,10 +4069,13 @@
       <c r="D167" t="s">
         <v>22</v>
       </c>
-      <c r="E167" s="0">
+      <c r="E167" t="s">
+        <v>52</v>
+      </c>
+      <c r="F167" s="0">
         <v>350</v>
       </c>
-      <c r="F167" s="0">
+      <c r="G167" s="0">
         <v>290</v>
       </c>
     </row>
@@ -3525,10 +4092,13 @@
       <c r="D168" t="s">
         <v>22</v>
       </c>
-      <c r="E168" s="0">
+      <c r="E168" t="s">
+        <v>52</v>
+      </c>
+      <c r="F168" s="0">
         <v>395</v>
       </c>
-      <c r="F168" s="0">
+      <c r="G168" s="0">
         <v>325</v>
       </c>
     </row>
@@ -3545,10 +4115,13 @@
       <c r="D169" t="s">
         <v>22</v>
       </c>
-      <c r="E169" s="0">
+      <c r="E169" t="s">
+        <v>51</v>
+      </c>
+      <c r="F169" s="0">
         <v>120</v>
       </c>
-      <c r="F169" s="0">
+      <c r="G169" s="0">
         <v>100</v>
       </c>
     </row>
@@ -3565,10 +4138,13 @@
       <c r="D170" t="s">
         <v>22</v>
       </c>
-      <c r="E170" s="0">
+      <c r="E170" t="s">
+        <v>52</v>
+      </c>
+      <c r="F170" s="0">
         <v>425</v>
       </c>
-      <c r="F170" s="0">
+      <c r="G170" s="0">
         <v>345</v>
       </c>
     </row>
@@ -3585,12 +4161,15 @@
       <c r="D171" t="s">
         <v>23</v>
       </c>
-      <c r="E171" s="0">
-        <v>20</v>
+      <c r="E171" t="s">
+        <v>37</v>
       </c>
       <c r="F171" s="0">
         <v>20</v>
       </c>
+      <c r="G171" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
@@ -3605,12 +4184,15 @@
       <c r="D172" t="s">
         <v>23</v>
       </c>
-      <c r="E172" s="0">
-        <v>5</v>
+      <c r="E172" t="s">
+        <v>37</v>
       </c>
       <c r="F172" s="0">
         <v>5</v>
       </c>
+      <c r="G172" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
@@ -3625,12 +4207,15 @@
       <c r="D173" t="s">
         <v>23</v>
       </c>
-      <c r="E173" s="0">
-        <v>10</v>
+      <c r="E173" t="s">
+        <v>37</v>
       </c>
       <c r="F173" s="0">
         <v>10</v>
       </c>
+      <c r="G173" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
@@ -3645,12 +4230,15 @@
       <c r="D174" t="s">
         <v>23</v>
       </c>
-      <c r="E174" s="0">
-        <v>10</v>
+      <c r="E174" t="s">
+        <v>37</v>
       </c>
       <c r="F174" s="0">
         <v>10</v>
       </c>
+      <c r="G174" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
@@ -3665,10 +4253,13 @@
       <c r="D175" t="s">
         <v>12</v>
       </c>
-      <c r="E175" s="0">
+      <c r="E175" t="s">
+        <v>44</v>
+      </c>
+      <c r="F175" s="0">
         <v>1685</v>
       </c>
-      <c r="F175" s="0">
+      <c r="G175" s="0">
         <v>1005</v>
       </c>
     </row>
@@ -3685,10 +4276,13 @@
       <c r="D176" t="s">
         <v>12</v>
       </c>
-      <c r="E176" s="0">
+      <c r="E176" t="s">
+        <v>44</v>
+      </c>
+      <c r="F176" s="0">
         <v>670</v>
       </c>
-      <c r="F176" s="0">
+      <c r="G176" s="0">
         <v>510</v>
       </c>
     </row>
@@ -3705,10 +4299,13 @@
       <c r="D177" t="s">
         <v>12</v>
       </c>
-      <c r="E177" s="0">
+      <c r="E177" t="s">
+        <v>44</v>
+      </c>
+      <c r="F177" s="0">
         <v>85</v>
       </c>
-      <c r="F177" s="0">
+      <c r="G177" s="0">
         <v>75</v>
       </c>
     </row>
@@ -3725,10 +4322,13 @@
       <c r="D178" t="s">
         <v>12</v>
       </c>
-      <c r="E178" s="0">
+      <c r="E178" t="s">
+        <v>53</v>
+      </c>
+      <c r="F178" s="0">
         <v>150</v>
       </c>
-      <c r="F178" s="0">
+      <c r="G178" s="0">
         <v>120</v>
       </c>
     </row>
@@ -3745,10 +4345,13 @@
       <c r="D179" t="s">
         <v>12</v>
       </c>
-      <c r="E179" s="0">
+      <c r="E179" t="s">
+        <v>53</v>
+      </c>
+      <c r="F179" s="0">
         <v>135</v>
       </c>
-      <c r="F179" s="0">
+      <c r="G179" s="0">
         <v>115</v>
       </c>
     </row>
@@ -3765,10 +4368,13 @@
       <c r="D180" t="s">
         <v>6</v>
       </c>
-      <c r="E180" s="0">
+      <c r="E180" t="s">
+        <v>54</v>
+      </c>
+      <c r="F180" s="0">
         <v>55</v>
       </c>
-      <c r="F180" s="0">
+      <c r="G180" s="0">
         <v>50</v>
       </c>
     </row>
@@ -3785,10 +4391,13 @@
       <c r="D181" t="s">
         <v>7</v>
       </c>
-      <c r="E181" s="0">
+      <c r="E181" t="s">
+        <v>48</v>
+      </c>
+      <c r="F181" s="0">
         <v>350</v>
       </c>
-      <c r="F181" s="0">
+      <c r="G181" s="0">
         <v>315</v>
       </c>
     </row>
@@ -3805,10 +4414,13 @@
       <c r="D182" t="s">
         <v>6</v>
       </c>
-      <c r="E182" s="0">
+      <c r="E182" t="s">
+        <v>54</v>
+      </c>
+      <c r="F182" s="0">
         <v>50</v>
       </c>
-      <c r="F182" s="0">
+      <c r="G182" s="0">
         <v>45</v>
       </c>
     </row>
@@ -3825,10 +4437,13 @@
       <c r="D183" t="s">
         <v>7</v>
       </c>
-      <c r="E183" s="0">
+      <c r="E183" t="s">
+        <v>48</v>
+      </c>
+      <c r="F183" s="0">
         <v>415</v>
       </c>
-      <c r="F183" s="0">
+      <c r="G183" s="0">
         <v>375</v>
       </c>
     </row>
@@ -3845,10 +4460,13 @@
       <c r="D184" t="s">
         <v>12</v>
       </c>
-      <c r="E184" s="0">
+      <c r="E184" t="s">
+        <v>53</v>
+      </c>
+      <c r="F184" s="0">
         <v>60</v>
       </c>
-      <c r="F184" s="0">
+      <c r="G184" s="0">
         <v>50</v>
       </c>
     </row>
@@ -3865,10 +4483,13 @@
       <c r="D185" t="s">
         <v>7</v>
       </c>
-      <c r="E185" s="0">
+      <c r="E185" t="s">
+        <v>55</v>
+      </c>
+      <c r="F185" s="0">
         <v>1235</v>
       </c>
-      <c r="F185" s="0">
+      <c r="G185" s="0">
         <v>1110</v>
       </c>
     </row>
@@ -3885,10 +4506,13 @@
       <c r="D186" t="s">
         <v>7</v>
       </c>
-      <c r="E186" s="0">
+      <c r="E186" t="s">
+        <v>55</v>
+      </c>
+      <c r="F186" s="0">
         <v>1265</v>
       </c>
-      <c r="F186" s="0">
+      <c r="G186" s="0">
         <v>1135</v>
       </c>
     </row>
@@ -3905,10 +4529,13 @@
       <c r="D187" t="s">
         <v>7</v>
       </c>
-      <c r="E187" s="0">
+      <c r="E187" t="s">
+        <v>55</v>
+      </c>
+      <c r="F187" s="0">
         <v>1280</v>
       </c>
-      <c r="F187" s="0">
+      <c r="G187" s="0">
         <v>1150</v>
       </c>
     </row>
@@ -3925,10 +4552,13 @@
       <c r="D188" t="s">
         <v>12</v>
       </c>
-      <c r="E188" s="0">
+      <c r="E188" t="s">
+        <v>53</v>
+      </c>
+      <c r="F188" s="0">
         <v>105</v>
       </c>
-      <c r="F188" s="0">
+      <c r="G188" s="0">
         <v>85</v>
       </c>
     </row>
@@ -3945,10 +4575,13 @@
       <c r="D189" t="s">
         <v>6</v>
       </c>
-      <c r="E189" s="0">
+      <c r="E189" t="s">
+        <v>54</v>
+      </c>
+      <c r="F189" s="0">
         <v>65</v>
       </c>
-      <c r="F189" s="0">
+      <c r="G189" s="0">
         <v>60</v>
       </c>
     </row>
@@ -3965,10 +4598,13 @@
       <c r="D190" t="s">
         <v>24</v>
       </c>
-      <c r="E190" s="0">
+      <c r="E190" t="s">
+        <v>37</v>
+      </c>
+      <c r="F190" s="0">
         <v>1305</v>
       </c>
-      <c r="F190" s="0">
+      <c r="G190" s="0">
         <v>1190</v>
       </c>
     </row>
@@ -3985,10 +4621,13 @@
       <c r="D191" t="s">
         <v>24</v>
       </c>
-      <c r="E191" s="0">
+      <c r="E191" t="s">
+        <v>37</v>
+      </c>
+      <c r="F191" s="0">
         <v>1045</v>
       </c>
-      <c r="F191" s="0">
+      <c r="G191" s="0">
         <v>965</v>
       </c>
     </row>
@@ -4005,10 +4644,13 @@
       <c r="D192" t="s">
         <v>19</v>
       </c>
-      <c r="E192" s="0">
+      <c r="E192" t="s">
+        <v>37</v>
+      </c>
+      <c r="F192" s="0">
         <v>75</v>
       </c>
-      <c r="F192" s="0">
+      <c r="G192" s="0">
         <v>70</v>
       </c>
     </row>
@@ -4025,10 +4667,13 @@
       <c r="D193" t="s">
         <v>19</v>
       </c>
-      <c r="E193" s="0">
+      <c r="E193" t="s">
+        <v>37</v>
+      </c>
+      <c r="F193" s="0">
         <v>75</v>
       </c>
-      <c r="F193" s="0">
+      <c r="G193" s="0">
         <v>70</v>
       </c>
     </row>
@@ -4045,10 +4690,13 @@
       <c r="D194" t="s">
         <v>19</v>
       </c>
-      <c r="E194" s="0">
+      <c r="E194" t="s">
+        <v>37</v>
+      </c>
+      <c r="F194" s="0">
         <v>45</v>
       </c>
-      <c r="F194" s="0">
+      <c r="G194" s="0">
         <v>35</v>
       </c>
     </row>
@@ -4065,12 +4713,15 @@
       <c r="D195" t="s">
         <v>19</v>
       </c>
-      <c r="E195" s="0">
-        <v>80</v>
+      <c r="E195" t="s">
+        <v>37</v>
       </c>
       <c r="F195" s="0">
         <v>80</v>
       </c>
+      <c r="G195" s="0">
+        <v>80</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
@@ -4085,12 +4736,15 @@
       <c r="D196" t="s">
         <v>25</v>
       </c>
-      <c r="E196" s="0">
-        <v>100</v>
+      <c r="E196" t="s">
+        <v>37</v>
       </c>
       <c r="F196" s="0">
         <v>100</v>
       </c>
+      <c r="G196" s="0">
+        <v>100</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
@@ -4105,10 +4759,13 @@
       <c r="D197" t="s">
         <v>26</v>
       </c>
-      <c r="E197" s="0">
+      <c r="E197" t="s">
+        <v>37</v>
+      </c>
+      <c r="F197" s="0">
         <v>305</v>
       </c>
-      <c r="F197" s="0">
+      <c r="G197" s="0">
         <v>290</v>
       </c>
     </row>
@@ -4125,12 +4782,15 @@
       <c r="D198" t="s">
         <v>19</v>
       </c>
-      <c r="E198" s="0">
-        <v>85</v>
+      <c r="E198" t="s">
+        <v>37</v>
       </c>
       <c r="F198" s="0">
         <v>85</v>
       </c>
+      <c r="G198" s="0">
+        <v>85</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
@@ -4145,10 +4805,13 @@
       <c r="D199" t="s">
         <v>25</v>
       </c>
-      <c r="E199" s="0">
+      <c r="E199" t="s">
+        <v>37</v>
+      </c>
+      <c r="F199" s="0">
         <v>130</v>
       </c>
-      <c r="F199" s="0">
+      <c r="G199" s="0">
         <v>125</v>
       </c>
     </row>
@@ -4165,10 +4828,13 @@
       <c r="D200" t="s">
         <v>25</v>
       </c>
-      <c r="E200" s="0">
+      <c r="E200" t="s">
+        <v>37</v>
+      </c>
+      <c r="F200" s="0">
         <v>130</v>
       </c>
-      <c r="F200" s="0">
+      <c r="G200" s="0">
         <v>120</v>
       </c>
     </row>
@@ -4185,12 +4851,15 @@
       <c r="D201" t="s">
         <v>27</v>
       </c>
-      <c r="E201" s="0">
-        <v>15</v>
+      <c r="E201" t="s">
+        <v>37</v>
       </c>
       <c r="F201" s="0">
         <v>15</v>
       </c>
+      <c r="G201" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
@@ -4205,10 +4874,13 @@
       <c r="D202" t="s">
         <v>25</v>
       </c>
-      <c r="E202" s="0">
+      <c r="E202" t="s">
+        <v>37</v>
+      </c>
+      <c r="F202" s="0">
         <v>280</v>
       </c>
-      <c r="F202" s="0">
+      <c r="G202" s="0">
         <v>275</v>
       </c>
     </row>
@@ -4225,10 +4897,13 @@
       <c r="D203" t="s">
         <v>19</v>
       </c>
-      <c r="E203" s="0">
+      <c r="E203" t="s">
+        <v>37</v>
+      </c>
+      <c r="F203" s="0">
         <v>245</v>
       </c>
-      <c r="F203" s="0">
+      <c r="G203" s="0">
         <v>235</v>
       </c>
     </row>
@@ -4245,10 +4920,13 @@
       <c r="D204" t="s">
         <v>28</v>
       </c>
-      <c r="E204" s="0">
+      <c r="E204" t="s">
+        <v>56</v>
+      </c>
+      <c r="F204" s="0">
         <v>165</v>
       </c>
-      <c r="F204" s="0">
+      <c r="G204" s="0">
         <v>150</v>
       </c>
     </row>
@@ -4265,10 +4943,13 @@
       <c r="D205" t="s">
         <v>28</v>
       </c>
-      <c r="E205" s="0">
+      <c r="E205" t="s">
+        <v>56</v>
+      </c>
+      <c r="F205" s="0">
         <v>155</v>
       </c>
-      <c r="F205" s="0">
+      <c r="G205" s="0">
         <v>145</v>
       </c>
     </row>
@@ -4285,10 +4966,13 @@
       <c r="D206" t="s">
         <v>28</v>
       </c>
-      <c r="E206" s="0">
+      <c r="E206" t="s">
+        <v>56</v>
+      </c>
+      <c r="F206" s="0">
         <v>175</v>
       </c>
-      <c r="F206" s="0">
+      <c r="G206" s="0">
         <v>140</v>
       </c>
     </row>
@@ -4305,10 +4989,13 @@
       <c r="D207" t="s">
         <v>29</v>
       </c>
-      <c r="E207" s="0">
+      <c r="E207" t="s">
+        <v>37</v>
+      </c>
+      <c r="F207" s="0">
         <v>95</v>
       </c>
-      <c r="F207" s="0">
+      <c r="G207" s="0">
         <v>90</v>
       </c>
     </row>
@@ -4325,10 +5012,13 @@
       <c r="D208" t="s">
         <v>19</v>
       </c>
-      <c r="E208" s="0">
+      <c r="E208" t="s">
+        <v>37</v>
+      </c>
+      <c r="F208" s="0">
         <v>250</v>
       </c>
-      <c r="F208" s="0">
+      <c r="G208" s="0">
         <v>235</v>
       </c>
     </row>
@@ -4345,10 +5035,13 @@
       <c r="D209" t="s">
         <v>19</v>
       </c>
-      <c r="E209" s="0">
+      <c r="E209" t="s">
+        <v>37</v>
+      </c>
+      <c r="F209" s="0">
         <v>230</v>
       </c>
-      <c r="F209" s="0">
+      <c r="G209" s="0">
         <v>225</v>
       </c>
     </row>
@@ -4365,10 +5058,13 @@
       <c r="D210" t="s">
         <v>29</v>
       </c>
-      <c r="E210" s="0">
+      <c r="E210" t="s">
+        <v>37</v>
+      </c>
+      <c r="F210" s="0">
         <v>100</v>
       </c>
-      <c r="F210" s="0">
+      <c r="G210" s="0">
         <v>95</v>
       </c>
     </row>
@@ -4385,10 +5081,13 @@
       <c r="D211" t="s">
         <v>19</v>
       </c>
-      <c r="E211" s="0">
+      <c r="E211" t="s">
+        <v>37</v>
+      </c>
+      <c r="F211" s="0">
         <v>225</v>
       </c>
-      <c r="F211" s="0">
+      <c r="G211" s="0">
         <v>220</v>
       </c>
     </row>
@@ -4405,10 +5104,13 @@
       <c r="D212" t="s">
         <v>29</v>
       </c>
-      <c r="E212" s="0">
+      <c r="E212" t="s">
+        <v>37</v>
+      </c>
+      <c r="F212" s="0">
         <v>100</v>
       </c>
-      <c r="F212" s="0">
+      <c r="G212" s="0">
         <v>95</v>
       </c>
     </row>
@@ -4425,10 +5127,13 @@
       <c r="D213" t="s">
         <v>29</v>
       </c>
-      <c r="E213" s="0">
+      <c r="E213" t="s">
+        <v>37</v>
+      </c>
+      <c r="F213" s="0">
         <v>95</v>
       </c>
-      <c r="F213" s="0">
+      <c r="G213" s="0">
         <v>90</v>
       </c>
     </row>
@@ -4445,10 +5150,13 @@
       <c r="D214" t="s">
         <v>22</v>
       </c>
-      <c r="E214" s="0">
+      <c r="E214" t="s">
+        <v>51</v>
+      </c>
+      <c r="F214" s="0">
         <v>70</v>
       </c>
-      <c r="F214" s="0">
+      <c r="G214" s="0">
         <v>60</v>
       </c>
     </row>
@@ -4465,10 +5173,13 @@
       <c r="D215" t="s">
         <v>28</v>
       </c>
-      <c r="E215" s="0">
+      <c r="E215" t="s">
+        <v>56</v>
+      </c>
+      <c r="F215" s="0">
         <v>175</v>
       </c>
-      <c r="F215" s="0">
+      <c r="G215" s="0">
         <v>155</v>
       </c>
     </row>
@@ -4485,12 +5196,15 @@
       <c r="D216" t="s">
         <v>30</v>
       </c>
-      <c r="E216" s="0">
-        <v>5</v>
+      <c r="E216" t="s">
+        <v>37</v>
       </c>
       <c r="F216" s="0">
         <v>5</v>
       </c>
+      <c r="G216" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
@@ -4505,12 +5219,15 @@
       <c r="D217" t="s">
         <v>30</v>
       </c>
-      <c r="E217" s="0">
-        <v>5</v>
+      <c r="E217" t="s">
+        <v>37</v>
       </c>
       <c r="F217" s="0">
         <v>5</v>
       </c>
+      <c r="G217" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
@@ -4525,12 +5242,15 @@
       <c r="D218" t="s">
         <v>30</v>
       </c>
-      <c r="E218" s="0">
-        <v>5</v>
+      <c r="E218" t="s">
+        <v>37</v>
       </c>
       <c r="F218" s="0">
         <v>5</v>
       </c>
+      <c r="G218" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
@@ -4545,12 +5265,15 @@
       <c r="D219" t="s">
         <v>30</v>
       </c>
-      <c r="E219" s="0">
-        <v>5</v>
+      <c r="E219" t="s">
+        <v>37</v>
       </c>
       <c r="F219" s="0">
         <v>5</v>
       </c>
+      <c r="G219" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
@@ -4565,12 +5288,15 @@
       <c r="D220" t="s">
         <v>30</v>
       </c>
-      <c r="E220" s="0">
-        <v>5</v>
+      <c r="E220" t="s">
+        <v>37</v>
       </c>
       <c r="F220" s="0">
         <v>5</v>
       </c>
+      <c r="G220" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
@@ -4585,10 +5311,13 @@
       <c r="D221" t="s">
         <v>28</v>
       </c>
-      <c r="E221" s="0">
+      <c r="E221" t="s">
+        <v>56</v>
+      </c>
+      <c r="F221" s="0">
         <v>185</v>
       </c>
-      <c r="F221" s="0">
+      <c r="G221" s="0">
         <v>160</v>
       </c>
     </row>
@@ -4605,10 +5334,13 @@
       <c r="D222" t="s">
         <v>29</v>
       </c>
-      <c r="E222" s="0">
+      <c r="E222" t="s">
+        <v>37</v>
+      </c>
+      <c r="F222" s="0">
         <v>100</v>
       </c>
-      <c r="F222" s="0">
+      <c r="G222" s="0">
         <v>95</v>
       </c>
     </row>
@@ -4625,10 +5357,13 @@
       <c r="D223" t="s">
         <v>29</v>
       </c>
-      <c r="E223" s="0">
+      <c r="E223" t="s">
+        <v>37</v>
+      </c>
+      <c r="F223" s="0">
         <v>95</v>
       </c>
-      <c r="F223" s="0">
+      <c r="G223" s="0">
         <v>90</v>
       </c>
     </row>
@@ -4645,10 +5380,13 @@
       <c r="D224" t="s">
         <v>28</v>
       </c>
-      <c r="E224" s="0">
+      <c r="E224" t="s">
+        <v>56</v>
+      </c>
+      <c r="F224" s="0">
         <v>190</v>
       </c>
-      <c r="F224" s="0">
+      <c r="G224" s="0">
         <v>165</v>
       </c>
     </row>
@@ -4665,10 +5403,13 @@
       <c r="D225" t="s">
         <v>28</v>
       </c>
-      <c r="E225" s="0">
+      <c r="E225" t="s">
+        <v>57</v>
+      </c>
+      <c r="F225" s="0">
         <v>190</v>
       </c>
-      <c r="F225" s="0">
+      <c r="G225" s="0">
         <v>160</v>
       </c>
     </row>
@@ -4685,12 +5426,15 @@
       <c r="D226" t="s">
         <v>29</v>
       </c>
-      <c r="E226" s="0">
-        <v>10</v>
+      <c r="E226" t="s">
+        <v>37</v>
       </c>
       <c r="F226" s="0">
         <v>10</v>
       </c>
+      <c r="G226" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
@@ -4705,12 +5449,15 @@
       <c r="D227" t="s">
         <v>29</v>
       </c>
-      <c r="E227" s="0">
-        <v>10</v>
+      <c r="E227" t="s">
+        <v>37</v>
       </c>
       <c r="F227" s="0">
         <v>10</v>
       </c>
+      <c r="G227" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
@@ -4725,12 +5472,15 @@
       <c r="D228" t="s">
         <v>29</v>
       </c>
-      <c r="E228" s="0">
-        <v>10</v>
+      <c r="E228" t="s">
+        <v>37</v>
       </c>
       <c r="F228" s="0">
         <v>10</v>
       </c>
+      <c r="G228" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
@@ -4745,10 +5495,13 @@
       <c r="D229" t="s">
         <v>28</v>
       </c>
-      <c r="E229" s="0">
+      <c r="E229" t="s">
+        <v>57</v>
+      </c>
+      <c r="F229" s="0">
         <v>200</v>
       </c>
-      <c r="F229" s="0">
+      <c r="G229" s="0">
         <v>170</v>
       </c>
     </row>
@@ -4765,12 +5518,15 @@
       <c r="D230" t="s">
         <v>29</v>
       </c>
-      <c r="E230" s="0">
-        <v>10</v>
+      <c r="E230" t="s">
+        <v>37</v>
       </c>
       <c r="F230" s="0">
         <v>10</v>
       </c>
+      <c r="G230" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
@@ -4785,12 +5541,15 @@
       <c r="D231" t="s">
         <v>30</v>
       </c>
-      <c r="E231" s="0">
-        <v>5</v>
+      <c r="E231" t="s">
+        <v>37</v>
       </c>
       <c r="F231" s="0">
         <v>5</v>
       </c>
+      <c r="G231" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
@@ -4805,12 +5564,15 @@
       <c r="D232" t="s">
         <v>30</v>
       </c>
-      <c r="E232" s="0">
-        <v>5</v>
+      <c r="E232" t="s">
+        <v>37</v>
       </c>
       <c r="F232" s="0">
         <v>5</v>
       </c>
+      <c r="G232" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
@@ -4825,10 +5587,13 @@
       <c r="D233" t="s">
         <v>28</v>
       </c>
-      <c r="E233" s="0">
+      <c r="E233" t="s">
+        <v>57</v>
+      </c>
+      <c r="F233" s="0">
         <v>205</v>
       </c>
-      <c r="F233" s="0">
+      <c r="G233" s="0">
         <v>180</v>
       </c>
     </row>
@@ -4845,10 +5610,13 @@
       <c r="D234" t="s">
         <v>31</v>
       </c>
-      <c r="E234" s="0">
+      <c r="E234" t="s">
+        <v>37</v>
+      </c>
+      <c r="F234" s="0">
         <v>70</v>
       </c>
-      <c r="F234" s="0">
+      <c r="G234" s="0">
         <v>50</v>
       </c>
     </row>
@@ -4865,10 +5633,13 @@
       <c r="D235" t="s">
         <v>23</v>
       </c>
-      <c r="E235" s="0">
+      <c r="E235" t="s">
+        <v>37</v>
+      </c>
+      <c r="F235" s="0">
         <v>20</v>
       </c>
-      <c r="F235" s="0">
+      <c r="G235" s="0">
         <v>20</v>
       </c>
     </row>
@@ -4883,12 +5654,15 @@
       <c r="D236" t="s">
         <v>32</v>
       </c>
-      <c r="E236" s="0">
-        <v>40</v>
+      <c r="E236" t="s">
+        <v>37</v>
       </c>
       <c r="F236" s="0">
         <v>40</v>
       </c>
+      <c r="G236" s="0">
+        <v>40</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
@@ -4903,10 +5677,13 @@
       <c r="D237" t="s">
         <v>33</v>
       </c>
-      <c r="E237" s="0">
+      <c r="E237" t="s">
+        <v>37</v>
+      </c>
+      <c r="F237" s="0">
         <v>40</v>
       </c>
-      <c r="F237" s="0">
+      <c r="G237" s="0">
         <v>35</v>
       </c>
     </row>
@@ -4923,10 +5700,13 @@
       <c r="D238" t="s">
         <v>31</v>
       </c>
-      <c r="E238" s="0">
+      <c r="E238" t="s">
+        <v>37</v>
+      </c>
+      <c r="F238" s="0">
         <v>205</v>
       </c>
-      <c r="F238" s="0">
+      <c r="G238" s="0">
         <v>70</v>
       </c>
     </row>
@@ -4943,10 +5723,13 @@
       <c r="D239" t="s">
         <v>31</v>
       </c>
-      <c r="E239" s="0">
+      <c r="E239" t="s">
+        <v>37</v>
+      </c>
+      <c r="F239" s="0">
         <v>170</v>
       </c>
-      <c r="F239" s="0">
+      <c r="G239" s="0">
         <v>65</v>
       </c>
     </row>
@@ -4963,10 +5746,13 @@
       <c r="D240" t="s">
         <v>31</v>
       </c>
-      <c r="E240" s="0">
+      <c r="E240" t="s">
+        <v>37</v>
+      </c>
+      <c r="F240" s="0">
         <v>180</v>
       </c>
-      <c r="F240" s="0">
+      <c r="G240" s="0">
         <v>65</v>
       </c>
     </row>
@@ -4983,10 +5769,13 @@
       <c r="D241" t="s">
         <v>31</v>
       </c>
-      <c r="E241" s="0">
+      <c r="E241" t="s">
+        <v>37</v>
+      </c>
+      <c r="F241" s="0">
         <v>90</v>
       </c>
-      <c r="F241" s="0">
+      <c r="G241" s="0">
         <v>35</v>
       </c>
     </row>
@@ -5003,10 +5792,13 @@
       <c r="D242" t="s">
         <v>31</v>
       </c>
-      <c r="E242" s="0">
+      <c r="E242" t="s">
+        <v>37</v>
+      </c>
+      <c r="F242" s="0">
         <v>155</v>
       </c>
-      <c r="F242" s="0">
+      <c r="G242" s="0">
         <v>60</v>
       </c>
     </row>
@@ -5023,12 +5815,15 @@
       <c r="D243" t="s">
         <v>31</v>
       </c>
-      <c r="E243" s="0">
-        <v>15</v>
+      <c r="E243" t="s">
+        <v>37</v>
       </c>
       <c r="F243" s="0">
         <v>15</v>
       </c>
+      <c r="G243" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
@@ -5043,12 +5838,15 @@
       <c r="D244" t="s">
         <v>33</v>
       </c>
-      <c r="E244" s="0">
-        <v>10</v>
+      <c r="E244" t="s">
+        <v>37</v>
       </c>
       <c r="F244" s="0">
         <v>10</v>
       </c>
+      <c r="G244" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
@@ -5063,10 +5861,13 @@
       <c r="D245" t="s">
         <v>23</v>
       </c>
-      <c r="E245" s="0">
+      <c r="E245" t="s">
+        <v>37</v>
+      </c>
+      <c r="F245" s="0">
         <v>20</v>
       </c>
-      <c r="F245" s="0">
+      <c r="G245" s="0">
         <v>10</v>
       </c>
     </row>
@@ -5081,10 +5882,13 @@
       <c r="D246" t="s">
         <v>32</v>
       </c>
-      <c r="E246" s="0">
+      <c r="E246" t="s">
+        <v>37</v>
+      </c>
+      <c r="F246" s="0">
         <v>70</v>
       </c>
-      <c r="F246" s="0">
+      <c r="G246" s="0">
         <v>60</v>
       </c>
     </row>
@@ -5099,10 +5903,13 @@
       <c r="D247" t="s">
         <v>32</v>
       </c>
-      <c r="E247" s="0">
+      <c r="E247" t="s">
+        <v>37</v>
+      </c>
+      <c r="F247" s="0">
         <v>60</v>
       </c>
-      <c r="F247" s="0">
+      <c r="G247" s="0">
         <v>60</v>
       </c>
     </row>
@@ -5117,10 +5924,13 @@
       <c r="D248" t="s">
         <v>32</v>
       </c>
-      <c r="E248" s="0">
+      <c r="E248" t="s">
+        <v>37</v>
+      </c>
+      <c r="F248" s="0">
         <v>60</v>
       </c>
-      <c r="F248" s="0">
+      <c r="G248" s="0">
         <v>60</v>
       </c>
     </row>
@@ -5135,10 +5945,13 @@
       <c r="D249" t="s">
         <v>32</v>
       </c>
-      <c r="E249" s="0">
+      <c r="E249" t="s">
+        <v>37</v>
+      </c>
+      <c r="F249" s="0">
         <v>60</v>
       </c>
-      <c r="F249" s="0">
+      <c r="G249" s="0">
         <v>60</v>
       </c>
     </row>
@@ -5153,10 +5966,13 @@
       <c r="D250" t="s">
         <v>32</v>
       </c>
-      <c r="E250" s="0">
+      <c r="E250" t="s">
+        <v>37</v>
+      </c>
+      <c r="F250" s="0">
         <v>45</v>
       </c>
-      <c r="F250" s="0">
+      <c r="G250" s="0">
         <v>45</v>
       </c>
     </row>
@@ -5171,10 +5987,13 @@
       <c r="D251" t="s">
         <v>32</v>
       </c>
-      <c r="E251" s="0">
+      <c r="E251" t="s">
+        <v>37</v>
+      </c>
+      <c r="F251" s="0">
         <v>55</v>
       </c>
-      <c r="F251" s="0">
+      <c r="G251" s="0">
         <v>55</v>
       </c>
     </row>
@@ -5189,12 +6008,15 @@
       <c r="D252" t="s">
         <v>32</v>
       </c>
-      <c r="E252" s="0">
-        <v>40</v>
+      <c r="E252" t="s">
+        <v>37</v>
       </c>
       <c r="F252" s="0">
         <v>40</v>
       </c>
+      <c r="G252" s="0">
+        <v>40</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
@@ -5209,12 +6031,15 @@
       <c r="D253" t="s">
         <v>34</v>
       </c>
-      <c r="E253" s="0">
-        <v>10</v>
+      <c r="E253" t="s">
+        <v>37</v>
       </c>
       <c r="F253" s="0">
         <v>10</v>
       </c>
+      <c r="G253" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
@@ -5229,12 +6054,15 @@
       <c r="D254" t="s">
         <v>34</v>
       </c>
-      <c r="E254" s="0">
-        <v>10</v>
+      <c r="E254" t="s">
+        <v>37</v>
       </c>
       <c r="F254" s="0">
         <v>10</v>
       </c>
+      <c r="G254" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
@@ -5249,10 +6077,13 @@
       <c r="D255" t="s">
         <v>34</v>
       </c>
-      <c r="E255" s="0">
+      <c r="E255" t="s">
+        <v>37</v>
+      </c>
+      <c r="F255" s="0">
         <v>10</v>
       </c>
-      <c r="F255" s="0">
+      <c r="G255" s="0">
         <v>10</v>
       </c>
     </row>
@@ -5267,12 +6098,15 @@
       <c r="D256" t="s">
         <v>32</v>
       </c>
-      <c r="E256" s="0">
-        <v>30</v>
+      <c r="E256" t="s">
+        <v>37</v>
       </c>
       <c r="F256" s="0">
         <v>30</v>
       </c>
+      <c r="G256" s="0">
+        <v>30</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
@@ -5287,10 +6121,13 @@
       <c r="D257" t="s">
         <v>35</v>
       </c>
-      <c r="E257" s="0">
+      <c r="E257" t="s">
+        <v>37</v>
+      </c>
+      <c r="F257" s="0">
         <v>5</v>
       </c>
-      <c r="F257" s="0">
+      <c r="G257" s="0">
         <v>5</v>
       </c>
     </row>
@@ -5305,10 +6142,13 @@
       <c r="D258" t="s">
         <v>32</v>
       </c>
-      <c r="E258" s="0">
+      <c r="E258" t="s">
+        <v>37</v>
+      </c>
+      <c r="F258" s="0">
         <v>30</v>
       </c>
-      <c r="F258" s="0">
+      <c r="G258" s="0">
         <v>30</v>
       </c>
     </row>
@@ -5323,10 +6163,13 @@
       <c r="D259" t="s">
         <v>32</v>
       </c>
-      <c r="E259" s="0">
+      <c r="E259" t="s">
+        <v>37</v>
+      </c>
+      <c r="F259" s="0">
         <v>40</v>
       </c>
-      <c r="F259" s="0">
+      <c r="G259" s="0">
         <v>40</v>
       </c>
     </row>
@@ -5341,10 +6184,13 @@
       <c r="D260" t="s">
         <v>32</v>
       </c>
-      <c r="E260" s="0">
+      <c r="E260" t="s">
+        <v>37</v>
+      </c>
+      <c r="F260" s="0">
         <v>35</v>
       </c>
-      <c r="F260" s="0">
+      <c r="G260" s="0">
         <v>35</v>
       </c>
     </row>
@@ -5359,10 +6205,13 @@
       <c r="D261" t="s">
         <v>32</v>
       </c>
-      <c r="E261" s="0">
+      <c r="E261" t="s">
+        <v>37</v>
+      </c>
+      <c r="F261" s="0">
         <v>30</v>
       </c>
-      <c r="F261" s="0">
+      <c r="G261" s="0">
         <v>30</v>
       </c>
     </row>
@@ -5377,12 +6226,15 @@
       <c r="D262" t="s">
         <v>32</v>
       </c>
-      <c r="E262" s="0">
-        <v>30</v>
+      <c r="E262" t="s">
+        <v>37</v>
       </c>
       <c r="F262" s="0">
         <v>30</v>
       </c>
+      <c r="G262" s="0">
+        <v>30</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
@@ -5397,10 +6249,13 @@
       <c r="D263" t="s">
         <v>30</v>
       </c>
-      <c r="E263" s="0">
+      <c r="E263" t="s">
+        <v>37</v>
+      </c>
+      <c r="F263" s="0">
         <v>15</v>
       </c>
-      <c r="F263" s="0">
+      <c r="G263" s="0">
         <v>15</v>
       </c>
     </row>
@@ -5415,10 +6270,13 @@
       <c r="D264" t="s">
         <v>32</v>
       </c>
-      <c r="E264" s="0">
+      <c r="E264" t="s">
+        <v>37</v>
+      </c>
+      <c r="F264" s="0">
         <v>35</v>
       </c>
-      <c r="F264" s="0">
+      <c r="G264" s="0">
         <v>35</v>
       </c>
     </row>
@@ -5433,10 +6291,13 @@
       <c r="D265" t="s">
         <v>32</v>
       </c>
-      <c r="E265" s="0">
+      <c r="E265" t="s">
+        <v>37</v>
+      </c>
+      <c r="F265" s="0">
         <v>35</v>
       </c>
-      <c r="F265" s="0">
+      <c r="G265" s="0">
         <v>35</v>
       </c>
     </row>
@@ -5451,10 +6312,13 @@
       <c r="D266" t="s">
         <v>32</v>
       </c>
-      <c r="E266" s="0">
+      <c r="E266" t="s">
+        <v>37</v>
+      </c>
+      <c r="F266" s="0">
         <v>30</v>
       </c>
-      <c r="F266" s="0">
+      <c r="G266" s="0">
         <v>30</v>
       </c>
     </row>
@@ -5469,12 +6333,15 @@
       <c r="D267" t="s">
         <v>32</v>
       </c>
-      <c r="E267" s="0">
-        <v>30</v>
+      <c r="E267" t="s">
+        <v>37</v>
       </c>
       <c r="F267" s="0">
         <v>30</v>
       </c>
+      <c r="G267" s="0">
+        <v>30</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
@@ -5489,10 +6356,13 @@
       <c r="D268" t="s">
         <v>19</v>
       </c>
-      <c r="E268" s="0">
+      <c r="E268" t="s">
+        <v>37</v>
+      </c>
+      <c r="F268" s="0">
         <v>110</v>
       </c>
-      <c r="F268" s="0">
+      <c r="G268" s="0">
         <v>100</v>
       </c>
     </row>
@@ -5509,10 +6379,13 @@
       <c r="D269" t="s">
         <v>19</v>
       </c>
-      <c r="E269" s="0">
+      <c r="E269" t="s">
+        <v>37</v>
+      </c>
+      <c r="F269" s="0">
         <v>120</v>
       </c>
-      <c r="F269" s="0">
+      <c r="G269" s="0">
         <v>110</v>
       </c>
     </row>
@@ -5529,10 +6402,13 @@
       <c r="D270" t="s">
         <v>19</v>
       </c>
-      <c r="E270" s="0">
+      <c r="E270" t="s">
+        <v>37</v>
+      </c>
+      <c r="F270" s="0">
         <v>145</v>
       </c>
-      <c r="F270" s="0">
+      <c r="G270" s="0">
         <v>135</v>
       </c>
     </row>
@@ -5549,10 +6425,13 @@
       <c r="D271" t="s">
         <v>19</v>
       </c>
-      <c r="E271" s="0">
+      <c r="E271" t="s">
+        <v>37</v>
+      </c>
+      <c r="F271" s="0">
         <v>155</v>
       </c>
-      <c r="F271" s="0">
+      <c r="G271" s="0">
         <v>145</v>
       </c>
     </row>
@@ -5813,9 +6692,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC61B238-4178-4D46-8163-D0A7C5FA0BE4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F60C241-E2BF-4602-93F1-A63F3193A05B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F663FF38-9D1B-4693-926A-82B473F5A418}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55E0EA5C-BDE7-4CC4-B84D-86BD4BA625DD}"/>
 </file>
</xml_diff>